<commit_message>
Actualizacion de la validacion del titulo del libro y el valor del libro
</commit_message>
<xml_diff>
--- a/datos/Data.xlsx
+++ b/datos/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENTOS USER\MUSICA\ScreenplayLibreriaNacional\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{368728EC-5F6C-4A57-9216-62428870DB80}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{38F5B54A-8205-4CAF-BB70-DB18CEBD55C1}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
     <workbookView windowHeight="11385" windowWidth="19350" xWindow="825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="1740"/>
   </bookViews>
@@ -36,19 +36,19 @@
     <t>ValorLibro</t>
   </si>
   <si>
-    <t>LA NOCHE EN QUE FRANKENSTEIN LEYO EL QUI...</t>
-  </si>
-  <si>
-    <t>$42,000</t>
-  </si>
-  <si>
-    <t>el principito</t>
-  </si>
-  <si>
-    <t>EL PRINCIPITO</t>
-  </si>
-  <si>
-    <t>$27,000</t>
+    <t>EL LIBRO DE LA ASTRONOMIA</t>
+  </si>
+  <si>
+    <t>$134,900</t>
+  </si>
+  <si>
+    <t>crimen y castigo</t>
+  </si>
+  <si>
+    <t>CRIMEN Y CASTIGO</t>
+  </si>
+  <si>
+    <t>$50,000</t>
   </si>
 </sst>
 </file>

</xml_diff>